<commit_message>
DBCP datasource closed twice
</commit_message>
<xml_diff>
--- a/test/MarkLogic-Hadoop Test Cases.xlsx
+++ b/test/MarkLogic-Hadoop Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/TopCoder/marklogic-hive-poc/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9F4C137A-37CD-2042-B9E1-D62BC955606F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DBA2B1BD-2269-984A-839A-EEF7902AC562}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="780" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Set 1" sheetId="1" r:id="rId1"/>
@@ -542,8 +542,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -592,7 +592,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="3">
-        <v>28671</v>
+        <v>28672</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -600,7 +600,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="3">
-        <v>1401641</v>
+        <v>1401640</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -672,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="3">
-        <v>19998</v>
+        <v>19999</v>
       </c>
       <c r="C14" s="3">
         <v>5465</v>
@@ -684,7 +684,7 @@
         <v>5465</v>
       </c>
       <c r="F14" s="3">
-        <v>19998</v>
+        <v>19999</v>
       </c>
       <c r="G14" s="3">
         <v>0</v>
@@ -698,10 +698,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3">
         <v>2</v>
@@ -718,7 +718,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="3">
-        <v>1220001</v>
+        <v>1220000</v>
       </c>
       <c r="C16" s="3">
         <v>45976</v>
@@ -730,7 +730,7 @@
         <v>45976</v>
       </c>
       <c r="F16" s="3">
-        <v>1220001</v>
+        <v>1220000</v>
       </c>
       <c r="G16" s="3">
         <v>45896</v>
@@ -744,7 +744,7 @@
         <v>180</v>
       </c>
       <c r="C17" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" s="3">
         <v>50</v>

</xml_diff>